<commit_message>
Add real resistor values of voltage divider (r1, r2)
</commit_message>
<xml_diff>
--- a/Energy consumption.xlsx
+++ b/Energy consumption.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Солнечная панель</t>
   </si>
@@ -45,9 +45,6 @@
     <t>3 А/ч</t>
   </si>
   <si>
-    <t>Энергопотребление</t>
-  </si>
-  <si>
     <t>STM32F103</t>
   </si>
   <si>
@@ -66,36 +63,18 @@
     <t>В сборе</t>
   </si>
   <si>
-    <t>80 мА</t>
-  </si>
-  <si>
-    <t>8 мА</t>
-  </si>
-  <si>
     <t>Сон</t>
   </si>
   <si>
-    <t>Ожидаемое время работы без подзарядки при батарее 2А/ч = 10 дней</t>
-  </si>
-  <si>
     <t>Стабилизатор</t>
   </si>
   <si>
     <t>всегда</t>
   </si>
   <si>
-    <t>4 мА</t>
-  </si>
-  <si>
     <t>6 с</t>
   </si>
   <si>
-    <t>5,2 мА</t>
-  </si>
-  <si>
-    <t>8,4 мА</t>
-  </si>
-  <si>
     <t>Sleep</t>
   </si>
   <si>
@@ -118,6 +97,15 @@
   </si>
   <si>
     <t>5mА</t>
+  </si>
+  <si>
+    <t>Энергопотребление (мА)</t>
+  </si>
+  <si>
+    <t>Ожидаемое время работы без подзарядки при батарее 2А/ч = 8,3 дней</t>
+  </si>
+  <si>
+    <t>Среднее энергопотребление = 10 мА</t>
   </si>
 </sst>
 </file>
@@ -653,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +701,7 @@
     </row>
     <row r="9" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -723,73 +711,92 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="18">
+        <v>5.2</v>
+      </c>
+      <c r="C11" s="10">
+        <v>8.4</v>
+      </c>
+      <c r="D11" s="10" t="str">
+        <f>D15</f>
+        <v>6 с</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f>D15</f>
+        <v>6 с</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="C13" s="14">
+        <v>70</v>
+      </c>
+      <c r="D13" s="10" t="str">
+        <f>D15</f>
+        <v>6 с</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="16">
+        <v>4</v>
+      </c>
+      <c r="C14" s="16">
+        <v>4</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="16">
+        <f>B11+B12+B13+B14</f>
+        <v>9.57</v>
+      </c>
+      <c r="C15" s="16">
+        <f>C11+C12+C13+C14</f>
+        <v>82.6</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -802,7 +809,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -810,10 +817,12 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -833,12 +842,12 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
       <c r="E22" s="28" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
@@ -846,47 +855,48 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E22:G22"/>
+    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add standby mode. Stable
Disable HAL_PWR_EnableWakeUpPin(PWR_WAKEUP_PIN1);
</commit_message>
<xml_diff>
--- a/Energy consumption.xlsx
+++ b/Energy consumption.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Солнечная панель</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Среднее энергопотребление = 10 мА</t>
+  </si>
+  <si>
+    <t>Зеленый светодиод 12мА</t>
+  </si>
+  <si>
+    <t>STM32</t>
+  </si>
+  <si>
+    <t>CS32</t>
   </si>
 </sst>
 </file>
@@ -165,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -281,11 +290,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,6 +387,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,10 +402,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -639,15 +700,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" customWidth="1"/>
@@ -692,211 +753,240 @@
       </c>
       <c r="C5" s="8"/>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="32">
+        <v>21.7</v>
+      </c>
+      <c r="C9" s="32">
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18">
-        <v>5.2</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B14" s="18"/>
+      <c r="C14" s="10">
         <v>8.4</v>
       </c>
-      <c r="D11" s="10" t="str">
-        <f>D15</f>
+      <c r="D14" s="10" t="str">
+        <f>D18</f>
         <v>6 с</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10">
         <v>0.2</v>
       </c>
-      <c r="D12" s="10" t="str">
-        <f>D15</f>
+      <c r="D15" s="10" t="str">
+        <f>D18</f>
         <v>6 с</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="C13" s="14">
-        <v>70</v>
-      </c>
-      <c r="D13" s="10" t="str">
-        <f>D15</f>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14">
+        <v>300</v>
+      </c>
+      <c r="D16" s="10" t="str">
+        <f>D18</f>
         <v>6 с</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16">
         <v>4</v>
       </c>
-      <c r="C14" s="16">
-        <v>4</v>
-      </c>
-      <c r="D14" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="16">
-        <f>B11+B12+B13+B14</f>
-        <v>9.57</v>
-      </c>
-      <c r="C15" s="16">
-        <f>C11+C12+C13+C14</f>
-        <v>82.6</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="B18" s="16">
+        <v>21.7</v>
+      </c>
+      <c r="C18" s="16">
+        <f>C14+C15+C16+C17</f>
+        <v>312.60000000000002</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
+      <c r="B25" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20" t="s">
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D26" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G26" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="A18:D18"/>
+  <mergeCells count="6">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>